<commit_message>
going to be done soon
</commit_message>
<xml_diff>
--- a/PORJECT/DOC-20240603-WA0004..xlsx
+++ b/PORJECT/DOC-20240603-WA0004..xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="177">
   <si>
     <t>THREADS AND CHALLENGES OF CYBER PHYSICAL SYSTEMS (CPS) AND DIGITAL TWINS (DT's)</t>
   </si>
@@ -35,7 +35,13 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>SR No.</t>
+  </si>
+  <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>Objective</t>
   </si>
   <si>
     <t>Threads</t>
@@ -200,7 +206,9 @@
     <t>Scability Issues in the Adoption of Digital Twins</t>
   </si>
   <si>
-    <t>We need to update Framework for DT Implementation at scale</t>
+    <t>We need to update Framework for DT Implementation at scale
+,Strategies for Enhanceing Interperability, Guidelines for  Regu
+latory compiance and Ethical use.</t>
   </si>
   <si>
     <t>Open and Smart Agile Cities</t>
@@ -212,13 +220,7 @@
     <t>Ineroprobility Between the Systems</t>
   </si>
   <si>
-    <t>,Strategies for Enhanceing Interperability, Guidelines for  Regu</t>
-  </si>
-  <si>
     <t>Regulatory and the Ethical considerations of DT's</t>
-  </si>
-  <si>
-    <t>latory compiance and Ethical use.</t>
   </si>
   <si>
     <t>CPS Security Area Issue 1.0</t>
@@ -240,7 +242,9 @@
 training, incident response planning, and researchto stay ahead of threats are essential.</t>
   </si>
   <si>
-    <t>Implement strong authentication, regular updates,</t>
+    <t>Implement strong authentication, regular updates,
+, encryption, intrusion detection systems, and industry
+collaboration for standardized security protocols​</t>
   </si>
   <si>
     <t>Santa Cruz</t>
@@ -249,12 +253,6 @@
     <t>insider threats</t>
   </si>
   <si>
-    <t>, encryption, intrusion detection systems, and industry</t>
-  </si>
-  <si>
-    <t>collaboration for standardized security protocols​</t>
-  </si>
-  <si>
     <t>Cyber-Physical Systems: A Confluence of Cutting Edge Technological Streams</t>
   </si>
   <si>
@@ -267,10 +265,18 @@
     <t xml:space="preserve">Key challenges include device heterogeneity, real-time operation </t>
   </si>
   <si>
-    <t>Conduct threat modeling,</t>
-  </si>
-  <si>
-    <t>Implement strong authentication, data encryption, continuous</t>
+    <t>Conduct threat modeling,
+risk assessments,
+security audits, penetratio
+n testing, and training
+programs. Develop
+AI-based threat detection,
+establish incident response plans.</t>
+  </si>
+  <si>
+    <t>Implement strong authentication, data encryption, continuous
+monitoring, intrusion detection and prevention systems
+regular updates, and industry collaboration.</t>
   </si>
   <si>
     <t>Bharat Bhargava</t>
@@ -282,33 +288,9 @@
     <t xml:space="preserve">requirements, interoperability, and maintaining security without </t>
   </si>
   <si>
-    <t>risk assessments,</t>
-  </si>
-  <si>
-    <t>monitoring, intrusion detection and prevention systems</t>
-  </si>
-  <si>
     <t>compromising performance.</t>
   </si>
   <si>
-    <t>security audits, penetratio</t>
-  </si>
-  <si>
-    <t>regular updates, and industry collaboration.</t>
-  </si>
-  <si>
-    <t>n testing, and training</t>
-  </si>
-  <si>
-    <t>programs. Develop</t>
-  </si>
-  <si>
-    <t>AI-based threat detection,</t>
-  </si>
-  <si>
-    <t>establish incident response plans.</t>
-  </si>
-  <si>
     <t>Digital Twin Modelling for Eco-Cyber-Physical</t>
   </si>
   <si>
@@ -324,10 +306,18 @@
     <t>Rapid environmental changes</t>
   </si>
   <si>
-    <t>Establish Living Labs</t>
-  </si>
-  <si>
-    <t>Use Living Labs for testing</t>
+    <t>Establish Living Labs
+Expand 4EM for agriculture
+Design and implement DTs
+Conduct stakeholder sessions
+Organize field trials and demos</t>
+  </si>
+  <si>
+    <t>Use Living Labs for testing
+Apply 4EM methodologies
+Develop DTs for better decisions
+Field trials and evaluations
+Collaborate with stakeholders</t>
   </si>
   <si>
     <t>engagement in a living lab.</t>
@@ -336,39 +326,15 @@
     <t>Integrating traditional and modern tech</t>
   </si>
   <si>
-    <t>Expand 4EM for agriculture</t>
-  </si>
-  <si>
-    <t>Apply 4EM methodologies</t>
-  </si>
-  <si>
     <t>System resilience and security</t>
   </si>
   <si>
-    <t>Design and implement DTs</t>
-  </si>
-  <si>
-    <t>Develop DTs for better decisions</t>
-  </si>
-  <si>
     <t>Accurate data collection</t>
   </si>
   <si>
-    <t>Conduct stakeholder sessions</t>
-  </si>
-  <si>
-    <t>Field trials and evaluations</t>
-  </si>
-  <si>
     <t>Managing diverse stakeholder needs</t>
   </si>
   <si>
-    <t>Organize field trials and demos</t>
-  </si>
-  <si>
-    <t>Collaborate with stakeholders</t>
-  </si>
-  <si>
     <t>Securing Cyber-Physical Systems through Digital Twins</t>
   </si>
   <si>
@@ -378,13 +344,25 @@
     <t xml:space="preserve">Use digital twins to emulate CPS, detect malicious behavior, and ensure correct operation through </t>
   </si>
   <si>
-    <t>Increased attack surface</t>
-  </si>
-  <si>
-    <t>Generate digital twins</t>
-  </si>
-  <si>
-    <t>Develop digital twins from CPS specs</t>
+    <t>Increased attack surface
+Identifying weaknesses in specifications
+Non-disruptive security testing
+Continuous monitoring for abnormalities
+Integration of virtual and physical systems</t>
+  </si>
+  <si>
+    <t>Generate digital twins
+Implement and monitor security rules
+Operate in simulation and replication modes
+Compare physical and virtual device states
+Develop features for scenario analysis</t>
+  </si>
+  <si>
+    <t>Develop digital twins from CPS specs
+Use emulated networks for virtual devices
+Implement security rules for anomaly detection
+Analyze in isolated virtual environments
+Use CPS Twinning framework</t>
   </si>
   <si>
     <t>Andreas Ekelhart (SBA Research)</t>
@@ -393,42 +371,6 @@
     <t>virtual replicas.</t>
   </si>
   <si>
-    <t>Identifying weaknesses in specifications</t>
-  </si>
-  <si>
-    <t>Implement and monitor security rules</t>
-  </si>
-  <si>
-    <t>Use emulated networks for virtual devices</t>
-  </si>
-  <si>
-    <t>Non-disruptive security testing</t>
-  </si>
-  <si>
-    <t>Operate in simulation and replication modes</t>
-  </si>
-  <si>
-    <t>Implement security rules for anomaly detection</t>
-  </si>
-  <si>
-    <t>Continuous monitoring for abnormalities</t>
-  </si>
-  <si>
-    <t>Compare physical and virtual device states</t>
-  </si>
-  <si>
-    <t>Analyze in isolated virtual environments</t>
-  </si>
-  <si>
-    <t>Integration of virtual and physical systems</t>
-  </si>
-  <si>
-    <t>Develop features for scenario analysis</t>
-  </si>
-  <si>
-    <t>Use CPS Twinning framework</t>
-  </si>
-  <si>
     <t>Engineering Of Dogital Twins For Cyber Physical Systems</t>
   </si>
   <si>
@@ -472,6 +414,9 @@
   </si>
   <si>
     <t>Mohsen Attaran, Bilge Gokhan Celik</t>
+  </si>
+  <si>
+    <t>Conduct a literature review to explore how Digital Twins streamline intelligent</t>
   </si>
   <si>
     <t>The main threads discussed include the application of Digital Twins in healthcare, life sciences,
@@ -483,16 +428,14 @@
     <t>Challenges include data management, integration complexities, and the need for high computational power. The paper also mentions the difficulty in standardizing Digital Twin technologies across different industries and ensuring data security and privacy.</t>
   </si>
   <si>
-    <t xml:space="preserve">Standardized frameworks,  advancements in  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Literature review, analyzing technologies, exploring </t>
-  </si>
-  <si>
-    <t>data analytics, robust cybersecurity measures.</t>
-  </si>
-  <si>
-    <t>applications, continuous R&amp;D​</t>
+    <t>Literature review, analyzing technologies, exploring applications, continuous R&amp;D​</t>
+  </si>
+  <si>
+    <t>Standardized frameworks,  advancements in  
+data analytics, robust cybersecurity measures.</t>
+  </si>
+  <si>
+    <t>automation across industries​</t>
   </si>
   <si>
     <t>Internet of Things and Cyber-Physical Systems</t>
@@ -501,52 +444,271 @@
     <t>Amit Kumar Tyagi , N. Sreenath</t>
   </si>
   <si>
+    <t>Address critical challenges in medical cyber-physical systems (MCPS) and propose solutions​</t>
+  </si>
+  <si>
     <t>Applications in smart grid systems, medical devices, and smart vehicles</t>
   </si>
   <si>
     <t>Security, privacy, verification, validation, certification of devices​</t>
   </si>
   <si>
+    <t>Identifying challenges, proposing solutions, case studies, collaboration</t>
+  </si>
+  <si>
     <t>Secure communication protocols, access control</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifying challenges, proposing solutions, case studies, </t>
-  </si>
-  <si>
     <t>, redundancy strategies</t>
   </si>
   <si>
-    <t>collaboration</t>
-  </si>
-  <si>
     <t>Advancements and Challenges of Digital Twins in Industry</t>
   </si>
   <si>
     <t>Fei Tao</t>
   </si>
   <si>
+    <t>Provide an overview of advancements and challenges in implementing digital twins</t>
+  </si>
+  <si>
     <t>Adoption in manufacturing, healthcare, urban planning, integrating IoT and AI</t>
   </si>
   <si>
     <t>Technological barriers, high costs, skill gaps, regulatory challenges​</t>
   </si>
   <si>
-    <t>Cloud and edge computing, industry-academia ​</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrating with IoT and AI, developing use cases, pilot </t>
+    <t>Integrating with IoT and AI, developing use cases, pilot 
+projects, training programs</t>
+  </si>
+  <si>
+    <t>Cloud and edge computing, industry-academia ​
+collaboration, regulatory guidelines</t>
   </si>
   <si>
     <t>, He Zhang &amp; Chenyuan Zhang</t>
   </si>
   <si>
-    <t>collaboration, regulatory guidelines</t>
-  </si>
-  <si>
-    <t>projects, training programs</t>
-  </si>
-  <si>
     <t>Nature Computational Science</t>
+  </si>
+  <si>
+    <t>An In-Depth Analysis of Cyber-Physical Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyze security vulnerabilities of CPS and propose mitigation strategies using deep </t>
+  </si>
+  <si>
+    <t>The threads include the exploration of security challenges in CPS, focusing on machine learning
+algorithms for threat detection and response. The paper also discusses the importance of robust
+control systems and the integration of advanced security protocols to protect against cyber attacks​​.</t>
+  </si>
+  <si>
+    <t>Resilience against cyber attacks, real-time detection, robust control system</t>
+  </si>
+  <si>
+    <t>Developing security solutions, threat assessments, real-time 
+monitoring, multidisciplinary research</t>
+  </si>
+  <si>
+    <t>Advanced machine learning algorithmsresilient control systems, comprehensive ​cybersecurity frameworks</t>
+  </si>
+  <si>
+    <t>machine intelligence</t>
+  </si>
+  <si>
+    <t>Cyber-Physical Systems in the Context of Industry 4.0</t>
+  </si>
+  <si>
+    <t>To provide a comprehensive approach to CPS in Industry 4.0 by categorizing relevant topics and</t>
+  </si>
+  <si>
+    <t>This paper threads through different future scenarios to forecast potential developments in CPS. It
+examines how emerging technologies, educational strategies, and industry needs might intersect
+and evolve by 2030​</t>
+  </si>
+  <si>
+    <t>Heterogeneity and interdisciplinary nature of CPS making classification</t>
+  </si>
+  <si>
+    <t>The paper suggests adaptive educational 
+strategies that incorporate emerging technologies and interdisciplinary approaches. It also emphasizes
+the need for continuous collaboration between academia &amp;  industry to stay ahead of technological trends</t>
+  </si>
+  <si>
+    <t>Systematic literature review and qualitative content analysis​​.</t>
+  </si>
+  <si>
+    <t>analyzing the current research landscape​</t>
+  </si>
+  <si>
+    <t>difficult</t>
+  </si>
+  <si>
+    <t>Cyber-Physical Systems Research and Education in 2030</t>
+  </si>
+  <si>
+    <t>To explore future scenarios and strategies for CPS research and education by 2030</t>
+  </si>
+  <si>
+    <t>Predicting technological advancements and aligning education with​</t>
+  </si>
+  <si>
+    <t>Scenario planning, trend analysis, and strategic forecasting</t>
+  </si>
+  <si>
+    <t>industry needs</t>
+  </si>
+  <si>
+    <t>Cyber-Physical Systems Security: Limitations, Issues, and Future Trends</t>
+  </si>
+  <si>
+    <t>To review current limitations and issues in CPS security and outline future trends</t>
+  </si>
+  <si>
+    <t>Reviewing control strategies and architectures used in CPS across different domains​</t>
+  </si>
+  <si>
+    <t>Current security measures' vulnerability and complexity of securing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluating security frameworks, identifying vulnerabilities, and </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed solutions include the development </t>
+  </si>
+  <si>
+    <t>integrated systems</t>
+  </si>
+  <si>
+    <t>researching new technologies​</t>
+  </si>
+  <si>
+    <t>of advanced security protocols and algorithms,</t>
+  </si>
+  <si>
+    <t>enhanced encryption techniques, and the</t>
+  </si>
+  <si>
+    <t>integration of artificial intelligence to</t>
+  </si>
+  <si>
+    <t>Distributed Control of Cyber Physical System on Various Domains</t>
+  </si>
+  <si>
+    <t>detect and mitigate threats in real-time​</t>
+  </si>
+  <si>
+    <t>To critically review distributed control mechanisms of CPS across various domains​</t>
+  </si>
+  <si>
+    <t>This review threads through various control strategies and architectures used in CPS across</t>
+  </si>
+  <si>
+    <t>Ensuring reliable communication, synchronization, and system stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewing literature, analyzing control strategies, and suggesting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robust control architectures, improved communication protocols, </t>
+  </si>
+  <si>
+    <t>different application domains. It identifies common patterns, differences, and the effectiveness</t>
+  </si>
+  <si>
+    <t>practical implementation</t>
+  </si>
+  <si>
+    <t>and synchronization technologies.</t>
+  </si>
+  <si>
+    <t>of these control mechanisms</t>
+  </si>
+  <si>
+    <t>9 Advantages and Disadvantages of Digital Twin Technology</t>
+  </si>
+  <si>
+    <t>Investigate security threats in diverse applications of Digital Twin technology, focusing on industrial</t>
+  </si>
+  <si>
+    <t>Digital Twins enable two-way communication between physical and virtual worlds, allowing dynamic</t>
+  </si>
+  <si>
+    <t>Ensuring cybersecurity for Digital Twins is complex due to integration</t>
+  </si>
+  <si>
+    <t>Continuous development of algorithms, models,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop secure platforms and industry-wide standards, continuous </t>
+  </si>
+  <si>
+    <t>smart cities, agriculture, disaster management, and battlefield monitoring.</t>
+  </si>
+  <si>
+    <t>updates and real-time modifications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> into critical infrastructure and lack of standardization, increasing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and communication systems, active research in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monitoring, advanced security technologies, and AI integration to </t>
+  </si>
+  <si>
+    <t>vulnerability to cyber-attacks.</t>
+  </si>
+  <si>
+    <t>cyber-physical systems, and implementing</t>
+  </si>
+  <si>
+    <t>neutralize threats.</t>
+  </si>
+  <si>
+    <t>security measures.</t>
+  </si>
+  <si>
+    <t>Digital Twins And Digital Threads: The Future Of Customized Health</t>
+  </si>
+  <si>
+    <t>Create personalized patient models to improve diagnosis, treatment, and healthcare outcomes</t>
+  </si>
+  <si>
+    <t>Seamless integration of patient data across diagnosis and treatment stages, ensuring consistent and</t>
+  </si>
+  <si>
+    <t>Data privacy concerns, need for high-quality interoperable data,</t>
+  </si>
+  <si>
+    <t>Collecting and integrating patient data,</t>
+  </si>
+  <si>
+    <t>Enhance data security, develop interoperable data standards,</t>
+  </si>
+  <si>
+    <t>through advanced simulations.</t>
+  </si>
+  <si>
+    <t>accessible information for personalized care.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and ensuring digital twin models accuratelyrepresent patient conditions. </t>
+  </si>
+  <si>
+    <t>developing precise simulation models,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use advanced analytics and AI, andfoster collaboration among </t>
+  </si>
+  <si>
+    <t>and continuously updating digital</t>
+  </si>
+  <si>
+    <t>healthcare stakeholders.</t>
+  </si>
+  <si>
+    <t>twins with new data and medical insights.</t>
   </si>
 </sst>
 </file>
@@ -588,16 +750,16 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calisto MT"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calisto MT"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -766,7 +928,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -775,6 +937,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -806,6 +974,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,7 +1300,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1150,16 +1324,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1168,89 +1342,89 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1258,28 +1432,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1294,14 +1475,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1621,34 +1812,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:A80"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.4444444444444" customWidth="1"/>
-    <col min="2" max="2" width="87.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="62.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="42.1388888888889" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="2" max="2" width="34.4444444444444" customWidth="1"/>
+    <col min="3" max="4" width="87.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="62.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="42.1388888888889" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="8" max="8" width="58.4444444444444" customWidth="1"/>
+    <col min="13" max="13" width="49.2777777777778" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="73.8" spans="2:5">
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="73.8" spans="3:7">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="2" spans="3:4">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1667,601 +1861,913 @@
       <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="G3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" hidden="1"/>
-    <row r="5" ht="14.1" customHeight="1" spans="1:2">
-      <c r="A5" s="9" t="s">
+    <row r="5" ht="14.1" customHeight="1" spans="1:4">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" ht="13.5" customHeight="1" spans="2:4">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" ht="23.25" customHeight="1" spans="2:8">
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" ht="23.25" customHeight="1" spans="2:7">
+      <c r="B8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" ht="23.25" customHeight="1" spans="2:7">
+      <c r="B9" s="14"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" ht="23.25" customHeight="1" spans="2:7">
+      <c r="B10" s="14"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" ht="23.25" customHeight="1" spans="2:7">
+      <c r="B11" s="14"/>
+      <c r="E11" s="19"/>
+      <c r="G11" s="19"/>
+    </row>
+    <row r="12" spans="5:5">
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" ht="22.5" customHeight="1" spans="1:4">
+      <c r="A13" s="11">
+        <v>2</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" ht="22.5" customHeight="1" spans="2:8">
+      <c r="B14" s="20"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" ht="22.5" customHeight="1" spans="3:8">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="19"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" ht="22.5" customHeight="1" spans="3:8">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="19"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" ht="22.5" customHeight="1" spans="5:8">
+      <c r="E17" s="19"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" ht="22.5" customHeight="1" spans="5:8">
+      <c r="E18" s="19"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" ht="22.5" customHeight="1" spans="8:8">
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" ht="22.5" customHeight="1" spans="8:8">
+      <c r="H20" s="19"/>
+    </row>
+    <row r="22" ht="21.75" customHeight="1" spans="1:4">
+      <c r="A22" s="11">
+        <v>3</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" ht="21.75" customHeight="1" spans="2:8">
+      <c r="B23" s="20"/>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" ht="21.75" customHeight="1" spans="2:5">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" ht="21.75" customHeight="1" spans="5:5">
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" ht="21.75" customHeight="1"/>
+    <row r="27" spans="1:4">
+      <c r="A27" s="11">
+        <v>4</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="5:7">
+      <c r="E30" s="19"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="5:7">
+      <c r="E31" s="19"/>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="7:7">
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="19"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="11">
+        <v>5</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="11">
+        <v>6</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" t="s">
+        <v>52</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5">
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5">
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="11">
+        <v>7</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="11">
         <v>8</v>
       </c>
-      <c r="B5" s="10"/>
-    </row>
-    <row r="6" ht="13.5" customHeight="1" spans="1:2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-    </row>
-    <row r="7" ht="23.25" customHeight="1" spans="1:6">
-      <c r="A7" s="11" t="s">
+      <c r="B59" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" t="s">
+        <v>71</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" t="s">
+        <v>75</v>
+      </c>
+      <c r="E61" t="s">
+        <v>76</v>
+      </c>
+      <c r="G61" s="19"/>
+      <c r="H61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="5:8">
+      <c r="E62" t="s">
+        <v>78</v>
+      </c>
+      <c r="G62" s="19"/>
+      <c r="H62" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="7:8">
+      <c r="G63" s="19"/>
+      <c r="H63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7">
+      <c r="G64" s="19"/>
+    </row>
+    <row r="65" spans="7:7">
+      <c r="G65" s="19"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="11">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B67" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="M67" s="21"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" t="s">
+        <v>83</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G68" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="11">
         <v>10</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="B73" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="B74" t="s">
+        <v>90</v>
+      </c>
+      <c r="C74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" t="s">
+        <v>93</v>
+      </c>
+      <c r="G74" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8">
+      <c r="H75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="11">
         <v>11</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="B77" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="M77" s="21"/>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" t="s">
+        <v>98</v>
+      </c>
+      <c r="C78" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" t="s">
+        <v>100</v>
+      </c>
+      <c r="E78" t="s">
+        <v>101</v>
+      </c>
+      <c r="G78" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H78" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="11">
         <v>12</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="B82" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="M82" s="21"/>
+    </row>
+    <row r="83" spans="3:13">
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E83" t="s">
+        <v>109</v>
+      </c>
+      <c r="G83" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="H83" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="M83" s="21"/>
+    </row>
+    <row r="84" spans="3:13">
+      <c r="C84" t="s">
+        <v>112</v>
+      </c>
+      <c r="D84"/>
+      <c r="G84" s="21"/>
+      <c r="H84"/>
+      <c r="M84" s="21"/>
+    </row>
+    <row r="85" spans="7:7">
+      <c r="G85" s="21"/>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="11">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="B87" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+    </row>
+    <row r="88" spans="3:8">
+      <c r="C88" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E88" t="s">
+        <v>116</v>
+      </c>
+      <c r="G88" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H88" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5">
+      <c r="C89" t="s">
+        <v>119</v>
+      </c>
+      <c r="D89"/>
+      <c r="E89" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" ht="23.25" customHeight="1" spans="1:5">
-      <c r="A8" s="11" t="s">
+      <c r="B96" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="3:8">
+      <c r="C97" t="s">
+        <v>122</v>
+      </c>
+      <c r="D97" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E97" t="s">
+        <v>123</v>
+      </c>
+      <c r="G97" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="H97" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="5:8">
+      <c r="E98" t="s">
+        <v>125</v>
+      </c>
+      <c r="G98" s="26"/>
+      <c r="H98" s="21"/>
+    </row>
+    <row r="99" spans="7:8">
+      <c r="G99" s="26"/>
+      <c r="H99" s="21"/>
+    </row>
+    <row r="100" spans="7:8">
+      <c r="G100" s="26"/>
+      <c r="H100" s="21"/>
+    </row>
+    <row r="101" spans="7:8">
+      <c r="G101" s="26"/>
+      <c r="H101" s="21"/>
+    </row>
+    <row r="102" spans="7:8">
+      <c r="G102" s="26"/>
+      <c r="H102" s="21"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="11">
         <v>15</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" ht="23.25" customHeight="1" spans="1:5">
-      <c r="A9" s="11"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" ht="23.25" customHeight="1" spans="1:5">
-      <c r="A10" s="11"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" ht="23.25" customHeight="1" spans="1:5">
-      <c r="A11" s="11"/>
-      <c r="C11" s="16"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="3:3">
-      <c r="C12" s="16"/>
-    </row>
-    <row r="13" ht="22.5" customHeight="1" spans="1:2">
-      <c r="A13" s="17" t="s">
+      <c r="B103" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="21"/>
+    </row>
+    <row r="104" spans="3:8">
+      <c r="C104" t="s">
+        <v>127</v>
+      </c>
+      <c r="D104" t="s">
+        <v>128</v>
+      </c>
+      <c r="E104" t="s">
+        <v>129</v>
+      </c>
+      <c r="G104" t="s">
+        <v>130</v>
+      </c>
+      <c r="H104" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="5:8">
+      <c r="E105" t="s">
+        <v>132</v>
+      </c>
+      <c r="G105" t="s">
+        <v>133</v>
+      </c>
+      <c r="H105" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="106" spans="8:8">
+      <c r="H106" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="107" spans="8:8">
+      <c r="H107" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="11">
         <v>16</v>
       </c>
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" ht="22.5" customHeight="1" spans="1:6">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14" t="s">
+      <c r="B108" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="H108" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8">
+      <c r="C109" t="s">
+        <v>139</v>
+      </c>
+      <c r="D109" t="s">
+        <v>140</v>
+      </c>
+      <c r="E109" t="s">
+        <v>141</v>
+      </c>
+      <c r="G109" t="s">
+        <v>142</v>
+      </c>
+      <c r="H109" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="110" spans="4:8">
+      <c r="D110" t="s">
+        <v>144</v>
+      </c>
+      <c r="G110" t="s">
+        <v>145</v>
+      </c>
+      <c r="H110" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4">
+      <c r="D111" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="11">
         <v>17</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="B113" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+    </row>
+    <row r="114" spans="3:8">
+      <c r="C114" t="s">
+        <v>149</v>
+      </c>
+      <c r="D114" t="s">
+        <v>150</v>
+      </c>
+      <c r="E114" t="s">
+        <v>151</v>
+      </c>
+      <c r="G114" t="s">
+        <v>152</v>
+      </c>
+      <c r="H114" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8">
+      <c r="C115" t="s">
+        <v>154</v>
+      </c>
+      <c r="D115" t="s">
+        <v>155</v>
+      </c>
+      <c r="E115" t="s">
+        <v>156</v>
+      </c>
+      <c r="G115" t="s">
+        <v>157</v>
+      </c>
+      <c r="H115" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="116" spans="5:8">
+      <c r="E116" t="s">
+        <v>159</v>
+      </c>
+      <c r="G116" t="s">
+        <v>160</v>
+      </c>
+      <c r="H116" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7">
+      <c r="G117" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="11">
         <v>18</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" ht="22.5" customHeight="1" spans="2:6">
-      <c r="B15" s="14"/>
-      <c r="C15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" ht="22.5" customHeight="1" spans="2:6">
-      <c r="B16" s="14"/>
-      <c r="C16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" ht="22.5" customHeight="1" spans="3:6">
-      <c r="C17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" ht="22.5" customHeight="1" spans="3:6">
-      <c r="C18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" ht="22.5" customHeight="1" spans="6:6">
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" ht="22.5" customHeight="1" spans="6:6">
-      <c r="F20" s="16"/>
-    </row>
-    <row r="22" ht="21.75" customHeight="1" spans="1:2">
-      <c r="A22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" ht="21.75" customHeight="1" spans="1:6">
-      <c r="A23" s="17"/>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" ht="21.75" customHeight="1" spans="1:6">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" ht="21.75" customHeight="1" spans="3:6">
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" ht="21.75" customHeight="1"/>
-    <row r="27" spans="1:2">
-      <c r="A27" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="10"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6">
-      <c r="C30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5">
-      <c r="C31" s="16"/>
-      <c r="E31" s="16"/>
-    </row>
-    <row r="32" spans="5:5">
-      <c r="E32" s="16"/>
-    </row>
-    <row r="33" spans="5:5">
-      <c r="E33" s="16"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6">
-      <c r="C38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" t="s">
-        <v>52</v>
-      </c>
-      <c r="F38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="5:5">
-      <c r="E39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="5:5">
-      <c r="E40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="5:5">
-      <c r="E41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="5:5">
-      <c r="E42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="10"/>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="10"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>62</v>
-      </c>
-      <c r="E46" t="s">
-        <v>63</v>
-      </c>
-      <c r="F46" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
-      <c r="B47" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" t="s">
-        <v>67</v>
-      </c>
-      <c r="F47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6">
-      <c r="C48" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6">
-      <c r="C49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6">
-      <c r="C50" t="s">
-        <v>75</v>
-      </c>
-      <c r="E50" t="s">
-        <v>76</v>
-      </c>
-      <c r="F50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" s="10"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" t="s">
-        <v>82</v>
-      </c>
-      <c r="F53" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" t="s">
-        <v>87</v>
-      </c>
-      <c r="F54" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6">
-      <c r="C55" t="s">
-        <v>89</v>
-      </c>
-      <c r="E55" t="s">
-        <v>90</v>
-      </c>
-      <c r="F55" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="3:6">
-      <c r="C56" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6">
-      <c r="C57" t="s">
-        <v>95</v>
-      </c>
-      <c r="E57" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="10"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F60" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" t="s">
-        <v>105</v>
-      </c>
-      <c r="C61" t="s">
-        <v>106</v>
-      </c>
-      <c r="E61" s="16"/>
-      <c r="F61" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="3:6">
-      <c r="C62" t="s">
-        <v>108</v>
-      </c>
-      <c r="E62" s="16"/>
-      <c r="F62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="5:6">
-      <c r="E63" s="16"/>
-      <c r="F63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="5:5">
-      <c r="E64" s="16"/>
-    </row>
-    <row r="65" spans="5:5">
-      <c r="E65" s="16"/>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67" s="10"/>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E68" t="s">
-        <v>115</v>
-      </c>
-      <c r="F68" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="69" spans="5:6">
-      <c r="E69" t="s">
-        <v>117</v>
-      </c>
-      <c r="F69" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73" s="10"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74" t="s">
-        <v>122</v>
-      </c>
-      <c r="E74" t="s">
-        <v>123</v>
-      </c>
-      <c r="F74" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="75" spans="5:6">
-      <c r="E75" t="s">
-        <v>125</v>
-      </c>
-      <c r="F75" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B77" s="10"/>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" t="s">
-        <v>128</v>
-      </c>
-      <c r="B78" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" t="s">
-        <v>130</v>
-      </c>
-      <c r="E78" t="s">
-        <v>131</v>
-      </c>
-      <c r="F78" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" t="s">
-        <v>133</v>
-      </c>
-      <c r="E79" t="s">
-        <v>134</v>
-      </c>
-      <c r="F79" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>136</v>
+      <c r="B119" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+    </row>
+    <row r="120" spans="3:8">
+      <c r="C120" t="s">
+        <v>164</v>
+      </c>
+      <c r="D120" t="s">
+        <v>165</v>
+      </c>
+      <c r="E120" t="s">
+        <v>166</v>
+      </c>
+      <c r="G120" t="s">
+        <v>167</v>
+      </c>
+      <c r="H120" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8">
+      <c r="C121" t="s">
+        <v>169</v>
+      </c>
+      <c r="D121" t="s">
+        <v>170</v>
+      </c>
+      <c r="E121" t="s">
+        <v>171</v>
+      </c>
+      <c r="G121" t="s">
+        <v>172</v>
+      </c>
+      <c r="H121" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="122" spans="7:8">
+      <c r="G122" t="s">
+        <v>174</v>
+      </c>
+      <c r="H122" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7">
+      <c r="G123" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C68:C71"/>
+  <mergeCells count="38">
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="E60:E65"/>
-    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G28:G33"/>
+    <mergeCell ref="G36:G42"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="G53:G57"/>
+    <mergeCell ref="G60:G65"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="G83:G85"/>
+    <mergeCell ref="G88:G94"/>
+    <mergeCell ref="H14:H20"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="H46:H50"/>
+    <mergeCell ref="H53:H57"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="H83:H84"/>
+    <mergeCell ref="H97:H103"/>
+    <mergeCell ref="M67:M68"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="M82:M84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>